<commit_message>
budget test cases updated
</commit_message>
<xml_diff>
--- a/budget-web-tests/testdata/Anonymous.xlsx
+++ b/budget-web-tests/testdata/Anonymous.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="108">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -323,7 +323,19 @@
     <t>SYD</t>
   </si>
   <si>
-    <t>AuthenticateUserTestCases</t>
+    <t>Budget_RES_Domestic_PayLater_US</t>
+  </si>
+  <si>
+    <t>Budget_RES_G_typeCoupon__SMSCheckbox_IATA_PayLater_US</t>
+  </si>
+  <si>
+    <t>GUZZ007</t>
+  </si>
+  <si>
+    <t>Budget_RES _Digital wallet Uplift _Direct_modify flow_US</t>
+  </si>
+  <si>
+    <t>Budget_RES_Misc_Step1,2_Step4 _ErrorMsg_Validation_US</t>
   </si>
   <si>
     <t>Budget_Profile_RES_Incognito_PayLater_US</t>
@@ -334,13 +346,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,12 +361,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF444444"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -365,14 +381,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,7 +389,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,7 +404,76 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,7 +488,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -425,62 +503,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,13 +526,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,127 +604,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,7 +634,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,19 +646,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,6 +717,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -720,6 +755,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -731,6 +775,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,47 +817,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -810,148 +837,154 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1275,10 +1308,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BA16"/>
+  <dimension ref="A1:BA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BF8" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:BA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1448,7 +1481,7 @@
       </c>
     </row>
     <row r="2" spans="1:53">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2027,7 +2060,7 @@
       <c r="AF5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AG5" s="6">
         <v>112000000000</v>
       </c>
       <c r="AH5" s="1" t="s">
@@ -2158,7 +2191,7 @@
       <c r="V6" s="1">
         <v>9838234567</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="6">
         <v>342000000000000</v>
       </c>
       <c r="X6" s="1">
@@ -2319,7 +2352,7 @@
       <c r="V7" s="1">
         <v>9838234567</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="6">
         <v>342000000000000</v>
       </c>
       <c r="X7" s="1">
@@ -3154,7 +3187,7 @@
       <c r="AF12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="6">
         <v>112000000000</v>
       </c>
       <c r="AH12" s="1" t="s">
@@ -3562,7 +3595,7 @@
       <c r="G15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>97</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -3702,7 +3735,7 @@
       </c>
     </row>
     <row r="16" spans="1:53">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B16" t="s">
@@ -3859,6 +3892,811 @@
         <v>56</v>
       </c>
       <c r="BA16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V17" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V18" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V19" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1129</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>123</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>99022</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V20" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X20" s="1">
+        <v>1129</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>123</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>99022</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="V21" s="1">
+        <v>9838234567</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA21" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4041,11 +4879,9 @@
       </c>
     </row>
     <row r="2" spans="1:53">
-      <c r="A2" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>

</xml_diff>